<commit_message>
In Web.cs added StoreFileList()
</commit_message>
<xml_diff>
--- a/ArletteSchedules/fall 2019.xlsx
+++ b/ArletteSchedules/fall 2019.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="8" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Traditional!$A$1:$F$77</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Traditional!$A$1:$F$76</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Traditional!$1:$4</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="202">
   <si>
     <t>Electrical Measurements and Circuits Laboratory</t>
   </si>
@@ -311,9 +311,6 @@
     <t>EE3445-02</t>
   </si>
   <si>
-    <t>EE3810-03</t>
-  </si>
-  <si>
     <t>EE2450-05</t>
   </si>
   <si>
@@ -395,9 +392,6 @@
     <t>Systems Risk Analysis</t>
   </si>
   <si>
-    <t>Principles of Signal Compression</t>
-  </si>
-  <si>
     <t>Probability, Random Variable, and Random Processes</t>
   </si>
   <si>
@@ -530,12 +524,6 @@
     <t>KHC4077</t>
   </si>
   <si>
-    <t>ETC251/ETC252</t>
-  </si>
-  <si>
-    <t>EE3810-04</t>
-  </si>
-  <si>
     <t>Shahverdi</t>
   </si>
   <si>
@@ -548,18 +536,12 @@
     <t>ETC255G</t>
   </si>
   <si>
-    <t>Nye</t>
-  </si>
-  <si>
     <t>F 200-340PM</t>
   </si>
   <si>
     <t>KHLH1</t>
   </si>
   <si>
-    <t>Liu</t>
-  </si>
-  <si>
     <t>EE2450-03</t>
   </si>
   <si>
@@ -587,8 +569,65 @@
     <t>SH264/SH260</t>
   </si>
   <si>
+    <t>Karimlou</t>
+  </si>
+  <si>
+    <t>Thorburn</t>
+  </si>
+  <si>
+    <t>EE3810-05</t>
+  </si>
+  <si>
+    <t>Lee</t>
+  </si>
+  <si>
+    <t>Karuhaka</t>
+  </si>
+  <si>
+    <t>ETC252</t>
+  </si>
+  <si>
+    <t>Mondin</t>
+  </si>
+  <si>
+    <t>Rad</t>
+  </si>
+  <si>
+    <t>Emrani</t>
+  </si>
+  <si>
+    <t>Zhao</t>
+  </si>
+  <si>
+    <t>Harris</t>
+  </si>
+  <si>
+    <t>Zhang</t>
+  </si>
+  <si>
+    <t>Kim</t>
+  </si>
+  <si>
+    <t>Linker</t>
+  </si>
+  <si>
+    <t>Wang</t>
+  </si>
+  <si>
+    <t>Fragoso</t>
+  </si>
+  <si>
+    <t>EE3810-06</t>
+  </si>
+  <si>
+    <t>Wireless Communications</t>
+  </si>
+  <si>
+    <t>FA223</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">2/20/2019                                                                             </t>
+      <t xml:space="preserve">6/5/2019                                                                             </t>
     </r>
     <r>
       <rPr>
@@ -600,12 +639,15 @@
       <t xml:space="preserve">           FALL 2019 COURSE LIST</t>
     </r>
   </si>
+  <si>
+    <t>SH358B</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -683,17 +725,6 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="12"/>
       <name val="Cambria"/>
       <family val="1"/>
@@ -728,7 +759,8 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="10"/>
+      <b/>
+      <sz val="14"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -877,7 +909,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -970,77 +1002,62 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="16" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="14" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1365,10 +1382,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G84"/>
+  <dimension ref="A1:G83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70:XFD76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1384,61 +1401,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="54" t="s">
-        <v>127</v>
-      </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
+      <c r="A1" s="50" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
-        <v>187</v>
-      </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="50"/>
+      <c r="A3" s="44" t="s">
+        <v>200</v>
+      </c>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="46"/>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="51"/>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="53"/>
+      <c r="A4" s="47"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="49"/>
     </row>
     <row r="5" spans="1:7" s="7" customFormat="1" ht="22.35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="40" t="s">
+      <c r="E5" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="F5" s="43" t="s">
+      <c r="F5" s="39" t="s">
         <v>33</v>
       </c>
       <c r="G5" s="9"/>
@@ -1448,19 +1465,19 @@
         <v>53</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C6" s="15">
         <v>3</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E6" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="46" t="s">
-        <v>186</v>
+      <c r="F6" s="42" t="s">
+        <v>180</v>
       </c>
       <c r="G6" s="9"/>
     </row>
@@ -1474,12 +1491,14 @@
       <c r="C7" s="19">
         <v>1</v>
       </c>
-      <c r="D7" s="20"/>
+      <c r="D7" s="20" t="s">
+        <v>194</v>
+      </c>
       <c r="E7" s="20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F7" s="24" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G7" s="12"/>
     </row>
@@ -1493,12 +1512,14 @@
       <c r="C8" s="19">
         <v>1</v>
       </c>
-      <c r="D8" s="20"/>
+      <c r="D8" s="20" t="s">
+        <v>194</v>
+      </c>
       <c r="E8" s="20" t="s">
         <v>42</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G8" s="12"/>
     </row>
@@ -1517,7 +1538,7 @@
         <v>79</v>
       </c>
       <c r="F9" s="24" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G9" s="12"/>
     </row>
@@ -1532,13 +1553,13 @@
         <v>2</v>
       </c>
       <c r="D10" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="F10" s="24" t="s">
         <v>149</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>150</v>
-      </c>
-      <c r="F10" s="24" t="s">
-        <v>151</v>
       </c>
       <c r="G10" s="9"/>
     </row>
@@ -1553,13 +1574,13 @@
         <v>1</v>
       </c>
       <c r="D11" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="F11" s="24" t="s">
         <v>149</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>131</v>
-      </c>
-      <c r="F11" s="24" t="s">
-        <v>151</v>
       </c>
       <c r="G11" s="9"/>
     </row>
@@ -1574,13 +1595,13 @@
         <v>2</v>
       </c>
       <c r="D12" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="F12" s="24" t="s">
         <v>149</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>152</v>
-      </c>
-      <c r="F12" s="24" t="s">
-        <v>151</v>
       </c>
       <c r="G12" s="9"/>
     </row>
@@ -1595,13 +1616,13 @@
         <v>1</v>
       </c>
       <c r="D13" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="F13" s="24" t="s">
         <v>149</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="F13" s="24" t="s">
-        <v>151</v>
       </c>
       <c r="G13" s="9"/>
     </row>
@@ -1615,12 +1636,14 @@
       <c r="C14" s="19">
         <v>2</v>
       </c>
-      <c r="D14" s="20"/>
+      <c r="D14" s="20" t="s">
+        <v>195</v>
+      </c>
       <c r="E14" s="20" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F14" s="24" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G14" s="9"/>
     </row>
@@ -1634,12 +1657,14 @@
       <c r="C15" s="19">
         <v>1</v>
       </c>
-      <c r="D15" s="20"/>
+      <c r="D15" s="20" t="s">
+        <v>195</v>
+      </c>
       <c r="E15" s="20" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F15" s="24" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G15" s="9"/>
     </row>
@@ -1653,12 +1678,14 @@
       <c r="C16" s="19">
         <v>1</v>
       </c>
-      <c r="D16" s="20"/>
+      <c r="D16" s="20" t="s">
+        <v>168</v>
+      </c>
       <c r="E16" s="20" t="s">
         <v>35</v>
       </c>
       <c r="F16" s="24" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G16" s="9"/>
     </row>
@@ -1672,12 +1699,14 @@
       <c r="C17" s="19">
         <v>1</v>
       </c>
-      <c r="D17" s="20"/>
+      <c r="D17" s="20" t="s">
+        <v>193</v>
+      </c>
       <c r="E17" s="20" t="s">
         <v>42</v>
       </c>
       <c r="F17" s="24" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G17" s="9"/>
     </row>
@@ -1691,12 +1720,14 @@
       <c r="C18" s="19">
         <v>1</v>
       </c>
-      <c r="D18" s="20"/>
+      <c r="D18" s="20" t="s">
+        <v>193</v>
+      </c>
       <c r="E18" s="20" t="s">
         <v>79</v>
       </c>
       <c r="F18" s="24" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G18" s="9"/>
     </row>
@@ -1711,13 +1742,13 @@
         <v>2</v>
       </c>
       <c r="D19" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="F19" s="24" t="s">
         <v>149</v>
-      </c>
-      <c r="E19" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="F19" s="24" t="s">
-        <v>151</v>
       </c>
       <c r="G19" s="9"/>
     </row>
@@ -1732,19 +1763,19 @@
         <v>1</v>
       </c>
       <c r="D20" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="F20" s="24" t="s">
         <v>149</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>133</v>
-      </c>
-      <c r="F20" s="24" t="s">
-        <v>151</v>
       </c>
       <c r="G20" s="9"/>
     </row>
     <row r="21" spans="1:7" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B21" s="18" t="s">
         <v>1</v>
@@ -1752,18 +1783,20 @@
       <c r="C21" s="19">
         <v>2</v>
       </c>
-      <c r="D21" s="20"/>
+      <c r="D21" s="20" t="s">
+        <v>168</v>
+      </c>
       <c r="E21" s="20" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F21" s="24" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G21" s="9"/>
     </row>
     <row r="22" spans="1:7" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B22" s="18" t="s">
         <v>1</v>
@@ -1771,18 +1804,20 @@
       <c r="C22" s="19">
         <v>1</v>
       </c>
-      <c r="D22" s="20"/>
+      <c r="D22" s="20" t="s">
+        <v>168</v>
+      </c>
       <c r="E22" s="20" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F22" s="24" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G22" s="9"/>
     </row>
     <row r="23" spans="1:7" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B23" s="18" t="s">
         <v>1</v>
@@ -1790,18 +1825,20 @@
       <c r="C23" s="19">
         <v>2</v>
       </c>
-      <c r="D23" s="20"/>
+      <c r="D23" s="20" t="s">
+        <v>195</v>
+      </c>
       <c r="E23" s="20" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F23" s="24" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G23" s="9"/>
     </row>
     <row r="24" spans="1:7" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B24" s="18" t="s">
         <v>1</v>
@@ -1809,12 +1846,14 @@
       <c r="C24" s="19">
         <v>1</v>
       </c>
-      <c r="D24" s="20"/>
+      <c r="D24" s="20" t="s">
+        <v>195</v>
+      </c>
       <c r="E24" s="20" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F24" s="24" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G24" s="9"/>
     </row>
@@ -1823,19 +1862,19 @@
         <v>58</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C25" s="19">
         <v>3</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E25" s="20" t="s">
         <v>36</v>
       </c>
       <c r="F25" s="24" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="G25" s="9"/>
     </row>
@@ -1849,18 +1888,20 @@
       <c r="C26" s="19">
         <v>1</v>
       </c>
-      <c r="D26" s="20"/>
+      <c r="D26" s="20" t="s">
+        <v>192</v>
+      </c>
       <c r="E26" s="20" t="s">
         <v>37</v>
       </c>
       <c r="F26" s="25" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G26" s="8"/>
     </row>
     <row r="27" spans="1:7" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="45" t="s">
-        <v>146</v>
+      <c r="A27" s="41" t="s">
+        <v>144</v>
       </c>
       <c r="B27" s="18" t="s">
         <v>4</v>
@@ -1873,13 +1914,13 @@
         <v>46</v>
       </c>
       <c r="F27" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="G27" s="8"/>
+    </row>
+    <row r="28" spans="1:7" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="41" t="s">
         <v>145</v>
-      </c>
-      <c r="G27" s="8"/>
-    </row>
-    <row r="28" spans="1:7" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="45" t="s">
-        <v>147</v>
       </c>
       <c r="B28" s="18" t="s">
         <v>4</v>
@@ -1892,13 +1933,13 @@
         <v>45</v>
       </c>
       <c r="F28" s="24" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G28" s="8"/>
     </row>
     <row r="29" spans="1:7" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="45" t="s">
-        <v>148</v>
+      <c r="A29" s="41" t="s">
+        <v>146</v>
       </c>
       <c r="B29" s="18" t="s">
         <v>4</v>
@@ -1911,7 +1952,7 @@
         <v>48</v>
       </c>
       <c r="F29" s="24" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G29" s="8"/>
     </row>
@@ -1920,19 +1961,19 @@
         <v>60</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C30" s="19">
         <v>3</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E30" s="20" t="s">
         <v>52</v>
       </c>
       <c r="F30" s="24" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G30" s="10"/>
     </row>
@@ -1941,19 +1982,19 @@
         <v>61</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C31" s="19">
         <v>3</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E31" s="20" t="s">
         <v>39</v>
       </c>
       <c r="F31" s="24" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G31" s="10"/>
     </row>
@@ -1968,13 +2009,13 @@
         <v>3</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E32" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="F32" s="24" t="s">
-        <v>144</v>
+      <c r="F32" s="43" t="s">
+        <v>201</v>
       </c>
       <c r="G32" s="10"/>
     </row>
@@ -1989,13 +2030,13 @@
         <v>1</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E33" s="20" t="s">
         <v>41</v>
       </c>
       <c r="F33" s="24" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G33" s="9"/>
     </row>
@@ -2009,29 +2050,29 @@
       <c r="G36" s="9"/>
     </row>
     <row r="37" spans="1:7" s="6" customFormat="1" ht="22.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="35" t="s">
+      <c r="A37" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="B37" s="36" t="s">
+      <c r="B37" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="C37" s="36" t="s">
+      <c r="C37" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="D37" s="36" t="s">
+      <c r="D37" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="E37" s="36" t="s">
+      <c r="E37" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="F37" s="37" t="s">
+      <c r="F37" s="33" t="s">
         <v>33</v>
       </c>
       <c r="G37" s="9"/>
     </row>
     <row r="38" spans="1:7" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="17" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B38" s="18" t="s">
         <v>5</v>
@@ -2039,18 +2080,20 @@
       <c r="C38" s="19">
         <v>3</v>
       </c>
-      <c r="D38" s="20"/>
+      <c r="D38" s="20" t="s">
+        <v>188</v>
+      </c>
       <c r="E38" s="20" t="s">
         <v>34</v>
       </c>
       <c r="F38" s="24" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G38" s="9"/>
     </row>
     <row r="39" spans="1:7" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="17" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B39" s="18" t="s">
         <v>5</v>
@@ -2058,18 +2101,20 @@
       <c r="C39" s="19">
         <v>3</v>
       </c>
-      <c r="D39" s="20"/>
+      <c r="D39" s="20" t="s">
+        <v>188</v>
+      </c>
       <c r="E39" s="20" t="s">
         <v>49</v>
       </c>
       <c r="F39" s="24" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G39" s="9"/>
     </row>
     <row r="40" spans="1:7" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="17" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B40" s="18" t="s">
         <v>6</v>
@@ -2077,12 +2122,14 @@
       <c r="C40" s="19">
         <v>1</v>
       </c>
-      <c r="D40" s="20"/>
+      <c r="D40" s="20" t="s">
+        <v>196</v>
+      </c>
       <c r="E40" s="20" t="s">
         <v>42</v>
       </c>
       <c r="F40" s="24" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G40" s="9"/>
     </row>
@@ -2097,13 +2144,13 @@
         <v>3</v>
       </c>
       <c r="D41" s="20" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E41" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="F41" s="24" t="s">
-        <v>182</v>
+      <c r="F41" s="43" t="s">
+        <v>199</v>
       </c>
       <c r="G41" s="9"/>
     </row>
@@ -2118,89 +2165,97 @@
         <v>3</v>
       </c>
       <c r="D42" s="20" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E42" s="20" t="s">
         <v>40</v>
       </c>
       <c r="F42" s="24" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G42" s="9"/>
     </row>
     <row r="43" spans="1:7" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="B43" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="B43" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="C43" s="39">
+      <c r="C43" s="35">
         <v>2</v>
       </c>
-      <c r="D43" s="20"/>
+      <c r="D43" s="20" t="s">
+        <v>168</v>
+      </c>
       <c r="E43" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="F43" s="44" t="s">
-        <v>151</v>
+        <v>162</v>
+      </c>
+      <c r="F43" s="40" t="s">
+        <v>149</v>
       </c>
       <c r="G43" s="9"/>
     </row>
     <row r="44" spans="1:7" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B44" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="C44" s="39">
+        <v>112</v>
+      </c>
+      <c r="C44" s="35">
         <v>1</v>
       </c>
-      <c r="D44" s="20"/>
+      <c r="D44" s="20" t="s">
+        <v>168</v>
+      </c>
       <c r="E44" s="20" t="s">
-        <v>165</v>
-      </c>
-      <c r="F44" s="44" t="s">
-        <v>151</v>
+        <v>163</v>
+      </c>
+      <c r="F44" s="40" t="s">
+        <v>149</v>
       </c>
       <c r="G44" s="9"/>
     </row>
     <row r="45" spans="1:7" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B45" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="C45" s="39">
+        <v>112</v>
+      </c>
+      <c r="C45" s="35">
         <v>2</v>
       </c>
-      <c r="D45" s="20"/>
+      <c r="D45" s="20" t="s">
+        <v>192</v>
+      </c>
       <c r="E45" s="20" t="s">
-        <v>166</v>
-      </c>
-      <c r="F45" s="44" t="s">
-        <v>151</v>
+        <v>164</v>
+      </c>
+      <c r="F45" s="40" t="s">
+        <v>149</v>
       </c>
       <c r="G45" s="9"/>
     </row>
     <row r="46" spans="1:7" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B46" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="C46" s="39">
+        <v>112</v>
+      </c>
+      <c r="C46" s="35">
         <v>1</v>
       </c>
-      <c r="D46" s="20"/>
+      <c r="D46" s="20" t="s">
+        <v>192</v>
+      </c>
       <c r="E46" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="F46" s="44" t="s">
-        <v>151</v>
+      <c r="F46" s="40" t="s">
+        <v>149</v>
       </c>
       <c r="G46" s="9"/>
     </row>
@@ -2214,12 +2269,14 @@
       <c r="C47" s="19">
         <v>1</v>
       </c>
-      <c r="D47" s="20"/>
+      <c r="D47" s="20" t="s">
+        <v>192</v>
+      </c>
       <c r="E47" s="20" t="s">
         <v>35</v>
       </c>
       <c r="F47" s="24" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G47" s="9"/>
     </row>
@@ -2233,12 +2290,14 @@
       <c r="C48" s="19">
         <v>3</v>
       </c>
-      <c r="D48" s="21"/>
+      <c r="D48" s="21" t="s">
+        <v>188</v>
+      </c>
       <c r="E48" s="21" t="s">
         <v>43</v>
       </c>
       <c r="F48" s="26" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G48" s="9"/>
     </row>
@@ -2253,13 +2312,13 @@
         <v>2</v>
       </c>
       <c r="D49" s="20" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E49" s="20" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F49" s="25" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G49" s="8"/>
     </row>
@@ -2273,39 +2332,41 @@
       <c r="C50" s="19">
         <v>1</v>
       </c>
-      <c r="D50" s="20"/>
+      <c r="D50" s="20" t="s">
+        <v>185</v>
+      </c>
       <c r="E50" s="20" t="s">
-        <v>133</v>
-      </c>
-      <c r="F50" s="47" t="s">
-        <v>168</v>
+        <v>131</v>
+      </c>
+      <c r="F50" s="25" t="s">
+        <v>136</v>
       </c>
       <c r="G50" s="8"/>
     </row>
     <row r="51" spans="1:7" s="6" customFormat="1" ht="30.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="17" t="s">
-        <v>95</v>
+        <v>183</v>
       </c>
       <c r="B51" s="18" t="s">
         <v>24</v>
       </c>
       <c r="C51" s="19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D51" s="20" t="s">
-        <v>139</v>
+        <v>185</v>
       </c>
       <c r="E51" s="20" t="s">
-        <v>132</v>
+        <v>35</v>
       </c>
       <c r="F51" s="25" t="s">
-        <v>167</v>
+        <v>186</v>
       </c>
       <c r="G51" s="8"/>
     </row>
     <row r="52" spans="1:7" s="6" customFormat="1" ht="30.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="17" t="s">
-        <v>169</v>
+        <v>197</v>
       </c>
       <c r="B52" s="18" t="s">
         <v>24</v>
@@ -2313,18 +2374,20 @@
       <c r="C52" s="19">
         <v>1</v>
       </c>
-      <c r="D52" s="20"/>
+      <c r="D52" s="20" t="s">
+        <v>184</v>
+      </c>
       <c r="E52" s="20" t="s">
-        <v>131</v>
-      </c>
-      <c r="F52" s="47" t="s">
-        <v>168</v>
+        <v>117</v>
+      </c>
+      <c r="F52" s="25" t="s">
+        <v>136</v>
       </c>
       <c r="G52" s="8"/>
     </row>
     <row r="53" spans="1:7" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B53" s="18" t="s">
         <v>10</v>
@@ -2332,12 +2395,14 @@
       <c r="C53" s="19">
         <v>3</v>
       </c>
-      <c r="D53" s="20"/>
+      <c r="D53" s="20" t="s">
+        <v>191</v>
+      </c>
       <c r="E53" s="20" t="s">
         <v>44</v>
       </c>
       <c r="F53" s="24" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G53" s="9"/>
     </row>
@@ -2351,12 +2416,14 @@
       <c r="C54" s="19">
         <v>3</v>
       </c>
-      <c r="D54" s="38"/>
+      <c r="D54" s="34" t="s">
+        <v>187</v>
+      </c>
       <c r="E54" s="20" t="s">
         <v>45</v>
       </c>
       <c r="F54" s="25" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="G54" s="9"/>
     </row>
@@ -2371,13 +2438,13 @@
         <v>3</v>
       </c>
       <c r="D55" s="20" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E55" s="20" t="s">
         <v>46</v>
       </c>
       <c r="F55" s="24" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G55" s="8"/>
     </row>
@@ -2392,13 +2459,13 @@
         <v>3</v>
       </c>
       <c r="D56" s="20" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E56" s="20" t="s">
         <v>48</v>
       </c>
       <c r="F56" s="24" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="G56" s="9"/>
     </row>
@@ -2413,13 +2480,13 @@
         <v>3</v>
       </c>
       <c r="D57" s="20" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E57" s="20" t="s">
         <v>39</v>
       </c>
       <c r="F57" s="24" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G57" s="9"/>
     </row>
@@ -2434,19 +2501,19 @@
         <v>3</v>
       </c>
       <c r="D58" s="20" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E58" s="20" t="s">
         <v>45</v>
       </c>
       <c r="F58" s="24" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G58" s="8"/>
     </row>
     <row r="59" spans="1:7" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B59" s="18" t="s">
         <v>16</v>
@@ -2454,18 +2521,20 @@
       <c r="C59" s="19">
         <v>3</v>
       </c>
-      <c r="D59" s="20"/>
+      <c r="D59" s="20" t="s">
+        <v>190</v>
+      </c>
       <c r="E59" s="20" t="s">
         <v>44</v>
       </c>
       <c r="F59" s="26" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G59" s="9"/>
     </row>
     <row r="60" spans="1:7" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B60" s="18" t="s">
         <v>18</v>
@@ -2474,19 +2543,19 @@
         <v>3</v>
       </c>
       <c r="D60" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E60" s="20" t="s">
         <v>38</v>
       </c>
       <c r="F60" s="24" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G60" s="9"/>
     </row>
     <row r="61" spans="1:7" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B61" s="18" t="s">
         <v>17</v>
@@ -2495,13 +2564,13 @@
         <v>3</v>
       </c>
       <c r="D61" s="20" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E61" s="20" t="s">
         <v>46</v>
       </c>
       <c r="F61" s="24" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G61" s="9"/>
     </row>
@@ -2510,17 +2579,19 @@
         <v>73</v>
       </c>
       <c r="B62" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C62" s="19">
         <v>3</v>
       </c>
-      <c r="D62" s="20"/>
+      <c r="D62" s="20" t="s">
+        <v>188</v>
+      </c>
       <c r="E62" s="20" t="s">
         <v>47</v>
       </c>
       <c r="F62" s="24" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="G62" s="9"/>
     </row>
@@ -2534,50 +2605,56 @@
       <c r="C63" s="19">
         <v>3</v>
       </c>
-      <c r="D63" s="20"/>
+      <c r="D63" s="20" t="s">
+        <v>189</v>
+      </c>
       <c r="E63" s="20" t="s">
         <v>48</v>
       </c>
       <c r="F63" s="26" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="G63" s="8"/>
     </row>
     <row r="64" spans="1:7" s="6" customFormat="1" ht="22.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B64" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C64" s="19">
         <v>1</v>
       </c>
-      <c r="D64" s="20"/>
+      <c r="D64" s="20" t="s">
+        <v>196</v>
+      </c>
       <c r="E64" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F64" s="26" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G64" s="8"/>
     </row>
     <row r="65" spans="1:7" s="6" customFormat="1" ht="22.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B65" s="18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C65" s="19">
         <v>3</v>
       </c>
-      <c r="D65" s="20"/>
+      <c r="D65" s="20" t="s">
+        <v>188</v>
+      </c>
       <c r="E65" s="20" t="s">
         <v>48</v>
       </c>
       <c r="F65" s="26" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G65" s="8"/>
     </row>
@@ -2592,17 +2669,35 @@
         <v>3</v>
       </c>
       <c r="D66" s="20" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E66" s="20" t="s">
         <v>43</v>
       </c>
       <c r="F66" s="24" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G66" s="8"/>
     </row>
     <row r="67" spans="1:7" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="B67" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C67" s="19">
+        <v>3</v>
+      </c>
+      <c r="D67" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="E67" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="F67" s="24" t="s">
+        <v>171</v>
+      </c>
       <c r="G67" s="8"/>
     </row>
     <row r="68" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -2613,225 +2708,212 @@
       <c r="G68" s="11"/>
     </row>
     <row r="69" spans="1:7" ht="22.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="35" t="s">
+      <c r="A69" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="B69" s="36" t="s">
+      <c r="B69" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="C69" s="36" t="s">
+      <c r="C69" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="D69" s="36" t="s">
+      <c r="D69" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="E69" s="36" t="s">
+      <c r="E69" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="F69" s="37" t="s">
+      <c r="F69" s="33" t="s">
         <v>33</v>
       </c>
       <c r="G69" s="11"/>
     </row>
-    <row r="70" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="B70" s="18" t="s">
-        <v>22</v>
+    <row r="70" spans="1:7" s="6" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="B70" s="23" t="s">
+        <v>121</v>
       </c>
       <c r="C70" s="19">
         <v>3</v>
       </c>
       <c r="D70" s="20" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="E70" s="20" t="s">
-        <v>175</v>
-      </c>
-      <c r="F70" s="24" t="s">
-        <v>176</v>
-      </c>
-      <c r="G70" s="11"/>
-    </row>
-    <row r="71" spans="1:7" s="6" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+      <c r="F70" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G70" s="8"/>
+    </row>
+    <row r="71" spans="1:7" s="6" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="22" t="s">
-        <v>121</v>
+        <v>76</v>
       </c>
       <c r="B71" s="23" t="s">
-        <v>122</v>
+        <v>25</v>
       </c>
       <c r="C71" s="19">
         <v>3</v>
       </c>
-      <c r="D71" s="20"/>
+      <c r="D71" s="34" t="s">
+        <v>187</v>
+      </c>
       <c r="E71" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="F71" s="25" t="s">
-        <v>137</v>
+        <v>48</v>
+      </c>
+      <c r="F71" s="24" t="s">
+        <v>169</v>
       </c>
       <c r="G71" s="8"/>
     </row>
-    <row r="72" spans="1:7" s="6" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="22" t="s">
-        <v>76</v>
+        <v>140</v>
       </c>
       <c r="B72" s="23" t="s">
-        <v>25</v>
+        <v>198</v>
       </c>
       <c r="C72" s="19">
         <v>3</v>
       </c>
-      <c r="D72" s="38"/>
+      <c r="D72" s="34" t="s">
+        <v>187</v>
+      </c>
       <c r="E72" s="20" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F72" s="24" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G72" s="8"/>
     </row>
-    <row r="73" spans="1:7" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="22" t="s">
-        <v>142</v>
+        <v>77</v>
       </c>
       <c r="B73" s="23" t="s">
-        <v>123</v>
+        <v>26</v>
       </c>
       <c r="C73" s="19">
         <v>3</v>
       </c>
-      <c r="D73" s="38"/>
+      <c r="D73" s="20" t="s">
+        <v>167</v>
+      </c>
       <c r="E73" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="F73" s="24" t="s">
-        <v>173</v>
+        <v>44</v>
+      </c>
+      <c r="F73" s="25" t="s">
+        <v>135</v>
       </c>
       <c r="G73" s="8"/>
     </row>
     <row r="74" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="22" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="B74" s="23" t="s">
-        <v>26</v>
+        <v>91</v>
       </c>
       <c r="C74" s="19">
         <v>3</v>
       </c>
       <c r="D74" s="20" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="E74" s="20" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="F74" s="25" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G74" s="8"/>
     </row>
     <row r="75" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="22" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="B75" s="23" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="C75" s="19">
         <v>3</v>
       </c>
       <c r="D75" s="20" t="s">
-        <v>170</v>
+        <v>190</v>
       </c>
       <c r="E75" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="F75" s="25" t="s">
-        <v>137</v>
+        <v>45</v>
+      </c>
+      <c r="F75" s="24" t="s">
+        <v>141</v>
       </c>
       <c r="G75" s="8"/>
     </row>
     <row r="76" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="22" t="s">
-        <v>107</v>
+        <v>78</v>
       </c>
       <c r="B76" s="23" t="s">
-        <v>101</v>
+        <v>27</v>
       </c>
       <c r="C76" s="19">
         <v>3</v>
       </c>
       <c r="D76" s="20" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="E76" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="F76" s="24" t="s">
-        <v>143</v>
+        <v>50</v>
+      </c>
+      <c r="F76" s="25" t="s">
+        <v>174</v>
       </c>
       <c r="G76" s="8"/>
     </row>
-    <row r="77" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="B77" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="C77" s="31">
-        <v>3</v>
-      </c>
-      <c r="D77" s="32"/>
-      <c r="E77" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="F77" s="25" t="s">
-        <v>180</v>
-      </c>
+    <row r="77" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
       <c r="G77" s="8"/>
     </row>
-    <row r="78" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
-      <c r="G78" s="8"/>
-    </row>
-    <row r="79" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C79" s="1"/>
-      <c r="D79" s="1"/>
-      <c r="E79" s="1"/>
-      <c r="F79" s="1"/>
+    </row>
+    <row r="79" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="37"/>
+      <c r="B79" s="29"/>
+      <c r="C79" s="30"/>
+      <c r="D79" s="30"/>
+      <c r="E79" s="29"/>
     </row>
     <row r="80" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="41"/>
-      <c r="B80" s="33"/>
-      <c r="C80" s="34"/>
-      <c r="D80" s="34"/>
-      <c r="E80" s="33"/>
+      <c r="A80" s="29"/>
+      <c r="B80" s="29"/>
+      <c r="C80" s="30"/>
+      <c r="D80" s="30"/>
+      <c r="E80" s="29"/>
     </row>
     <row r="81" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="33"/>
-      <c r="B81" s="33"/>
-      <c r="C81" s="34"/>
-      <c r="D81" s="34"/>
-      <c r="E81" s="33"/>
-    </row>
-    <row r="82" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="33"/>
-      <c r="B82" s="27"/>
-      <c r="C82" s="28"/>
-      <c r="D82" s="28"/>
-      <c r="E82" s="27"/>
-    </row>
-    <row r="83" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E83" s="1"/>
-    </row>
-    <row r="84" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="42"/>
+      <c r="A81" s="29"/>
+      <c r="B81" s="27"/>
+      <c r="C81" s="28"/>
+      <c r="D81" s="28"/>
+      <c r="E81" s="27"/>
+    </row>
+    <row r="82" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E82" s="1"/>
+    </row>
+    <row r="83" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="38"/>
     </row>
   </sheetData>
   <sortState ref="A6:L67">

</xml_diff>